<commit_message>
WIP copying results from excel to readme for React v16
</commit_message>
<xml_diff>
--- a/perf-results.xlsx
+++ b/perf-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28308"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="300" windowWidth="21040" windowHeight="19560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13900" yWindow="300" windowWidth="21040" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1143,7 +1143,7 @@
   </sheetPr>
   <dimension ref="A3:H39"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1967,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>